<commit_message>
Concurrency Modal và Web APIs
</commit_message>
<xml_diff>
--- a/me/2.Asynchronous-ProgrammingChương-Asynchronous-Programming/3.SetTimeout-va-nhung-hien-tuong-la.xlsx
+++ b/me/2.Asynchronous-ProgrammingChương-Asynchronous-Programming/3.SetTimeout-va-nhung-hien-tuong-la.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vudinhquang/Documents/quang/javascript_advance/me/2.Asynchronous-ProgrammingChương-Asynchronous-Programming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23EED1DD-FC04-3744-93FA-D267834BADE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6481A9EB-D86E-6C48-8BC6-9CB536D6A148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="1540" windowWidth="31900" windowHeight="17960" xr2:uid="{7DD41A9A-A940-8943-9205-0C46E49D1DCE}"/>
   </bookViews>
@@ -344,7 +344,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -355,7 +355,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -368,7 +367,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -383,7 +382,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1160,8 +1158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8FA5012-C009-0043-B961-62E649AB43CD}">
   <dimension ref="A3:I149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
-      <selection activeCell="E171" sqref="E171"/>
+    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
+      <selection activeCell="U138" sqref="U138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1178,12 +1176,9 @@
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B4" s="4"/>
-      <c r="C4" s="20" t="s">
+      <c r="C4" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
       <c r="G4" s="5"/>
       <c r="H4" t="s">
         <v>22</v>
@@ -1194,72 +1189,50 @@
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B5" s="4"/>
-      <c r="C5" s="20" t="s">
+      <c r="C5" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
       <c r="G5" s="5"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6" s="4"/>
-      <c r="C6" s="20" t="s">
+      <c r="C6" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
       <c r="G7" s="5"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="4"/>
-      <c r="C8" s="20" t="s">
+      <c r="C8" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B9" s="4"/>
-      <c r="C9" s="20" t="s">
+      <c r="C9" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
       <c r="G9" s="5"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B10" s="4"/>
-      <c r="C10" s="20" t="s">
+      <c r="C10" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B11" s="4"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20" t="s">
+      <c r="D11" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
@@ -1270,13 +1243,6 @@
       <c r="F12" s="8"/>
       <c r="G12" s="9"/>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-    </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>0</v>
@@ -1499,14 +1465,14 @@
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B91" s="4"/>
-      <c r="E91" s="10" t="s">
+      <c r="E91" t="s">
         <v>5</v>
       </c>
       <c r="G91" s="5"/>
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B92" s="4"/>
-      <c r="E92" s="10" t="s">
+      <c r="E92" t="s">
         <v>7</v>
       </c>
       <c r="G92" s="5"/>
@@ -1559,159 +1525,159 @@
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B100" s="11" t="s">
+      <c r="B100" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C100" s="12"/>
-      <c r="D100" s="12"/>
-      <c r="E100" s="12"/>
-      <c r="F100" s="12"/>
-      <c r="G100" s="12"/>
-      <c r="H100" s="13"/>
+      <c r="C100" s="11"/>
+      <c r="D100" s="11"/>
+      <c r="E100" s="11"/>
+      <c r="F100" s="11"/>
+      <c r="G100" s="11"/>
+      <c r="H100" s="12"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B101" s="14"/>
-      <c r="C101" s="15"/>
-      <c r="D101" s="15"/>
-      <c r="E101" s="15"/>
-      <c r="F101" s="15"/>
-      <c r="G101" s="15"/>
-      <c r="H101" s="16"/>
+      <c r="B101" s="13"/>
+      <c r="C101" s="14"/>
+      <c r="D101" s="14"/>
+      <c r="E101" s="14"/>
+      <c r="F101" s="14"/>
+      <c r="G101" s="14"/>
+      <c r="H101" s="15"/>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B102" s="14"/>
-      <c r="C102" s="15"/>
-      <c r="D102" s="15"/>
-      <c r="E102" s="15"/>
-      <c r="F102" s="15"/>
-      <c r="G102" s="15"/>
-      <c r="H102" s="16"/>
+      <c r="B102" s="13"/>
+      <c r="C102" s="14"/>
+      <c r="D102" s="14"/>
+      <c r="E102" s="14"/>
+      <c r="F102" s="14"/>
+      <c r="G102" s="14"/>
+      <c r="H102" s="15"/>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B103" s="14"/>
-      <c r="C103" s="15"/>
-      <c r="D103" s="15"/>
-      <c r="E103" s="15"/>
-      <c r="F103" s="15"/>
-      <c r="G103" s="15"/>
-      <c r="H103" s="16"/>
+      <c r="B103" s="13"/>
+      <c r="C103" s="14"/>
+      <c r="D103" s="14"/>
+      <c r="E103" s="14"/>
+      <c r="F103" s="14"/>
+      <c r="G103" s="14"/>
+      <c r="H103" s="15"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B104" s="14"/>
-      <c r="C104" s="15"/>
-      <c r="D104" s="15"/>
-      <c r="E104" s="15"/>
-      <c r="F104" s="15"/>
-      <c r="G104" s="15"/>
-      <c r="H104" s="16"/>
+      <c r="B104" s="13"/>
+      <c r="C104" s="14"/>
+      <c r="D104" s="14"/>
+      <c r="E104" s="14"/>
+      <c r="F104" s="14"/>
+      <c r="G104" s="14"/>
+      <c r="H104" s="15"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B105" s="14"/>
-      <c r="C105" s="15"/>
-      <c r="D105" s="15"/>
-      <c r="E105" s="15"/>
-      <c r="F105" s="15"/>
-      <c r="G105" s="15"/>
-      <c r="H105" s="16"/>
+      <c r="B105" s="13"/>
+      <c r="C105" s="14"/>
+      <c r="D105" s="14"/>
+      <c r="E105" s="14"/>
+      <c r="F105" s="14"/>
+      <c r="G105" s="14"/>
+      <c r="H105" s="15"/>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B106" s="14"/>
-      <c r="C106" s="15"/>
-      <c r="D106" s="15"/>
-      <c r="E106" s="15"/>
-      <c r="F106" s="15"/>
-      <c r="G106" s="15"/>
-      <c r="H106" s="16"/>
+      <c r="B106" s="13"/>
+      <c r="C106" s="14"/>
+      <c r="D106" s="14"/>
+      <c r="E106" s="14"/>
+      <c r="F106" s="14"/>
+      <c r="G106" s="14"/>
+      <c r="H106" s="15"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B107" s="14"/>
-      <c r="C107" s="15"/>
-      <c r="D107" s="15"/>
-      <c r="E107" s="15"/>
-      <c r="F107" s="15"/>
-      <c r="G107" s="15"/>
-      <c r="H107" s="16"/>
+      <c r="B107" s="13"/>
+      <c r="C107" s="14"/>
+      <c r="D107" s="14"/>
+      <c r="E107" s="14"/>
+      <c r="F107" s="14"/>
+      <c r="G107" s="14"/>
+      <c r="H107" s="15"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B108" s="14"/>
-      <c r="C108" s="15"/>
-      <c r="D108" s="15"/>
-      <c r="E108" s="15"/>
-      <c r="F108" s="15"/>
-      <c r="G108" s="15"/>
-      <c r="H108" s="16"/>
+      <c r="B108" s="13"/>
+      <c r="C108" s="14"/>
+      <c r="D108" s="14"/>
+      <c r="E108" s="14"/>
+      <c r="F108" s="14"/>
+      <c r="G108" s="14"/>
+      <c r="H108" s="15"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B109" s="14"/>
-      <c r="C109" s="15"/>
-      <c r="D109" s="15"/>
-      <c r="E109" s="15"/>
-      <c r="F109" s="15"/>
-      <c r="G109" s="15"/>
-      <c r="H109" s="16"/>
+      <c r="B109" s="13"/>
+      <c r="C109" s="14"/>
+      <c r="D109" s="14"/>
+      <c r="E109" s="14"/>
+      <c r="F109" s="14"/>
+      <c r="G109" s="14"/>
+      <c r="H109" s="15"/>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B110" s="14"/>
-      <c r="C110" s="15"/>
-      <c r="D110" s="15"/>
-      <c r="E110" s="15"/>
-      <c r="F110" s="15"/>
-      <c r="G110" s="15"/>
-      <c r="H110" s="16"/>
+      <c r="B110" s="13"/>
+      <c r="C110" s="14"/>
+      <c r="D110" s="14"/>
+      <c r="E110" s="14"/>
+      <c r="F110" s="14"/>
+      <c r="G110" s="14"/>
+      <c r="H110" s="15"/>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B111" s="14"/>
-      <c r="C111" s="15"/>
-      <c r="D111" s="15"/>
-      <c r="E111" s="15"/>
-      <c r="F111" s="15"/>
-      <c r="G111" s="15"/>
-      <c r="H111" s="16"/>
+      <c r="B111" s="13"/>
+      <c r="C111" s="14"/>
+      <c r="D111" s="14"/>
+      <c r="E111" s="14"/>
+      <c r="F111" s="14"/>
+      <c r="G111" s="14"/>
+      <c r="H111" s="15"/>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B112" s="14"/>
-      <c r="C112" s="15"/>
-      <c r="D112" s="15"/>
-      <c r="E112" s="15"/>
-      <c r="F112" s="15"/>
-      <c r="G112" s="15"/>
-      <c r="H112" s="16"/>
+      <c r="B112" s="13"/>
+      <c r="C112" s="14"/>
+      <c r="D112" s="14"/>
+      <c r="E112" s="14"/>
+      <c r="F112" s="14"/>
+      <c r="G112" s="14"/>
+      <c r="H112" s="15"/>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B113" s="14"/>
-      <c r="C113" s="15"/>
-      <c r="D113" s="15"/>
-      <c r="E113" s="15"/>
-      <c r="F113" s="15"/>
-      <c r="G113" s="15"/>
-      <c r="H113" s="16"/>
+      <c r="B113" s="13"/>
+      <c r="C113" s="14"/>
+      <c r="D113" s="14"/>
+      <c r="E113" s="14"/>
+      <c r="F113" s="14"/>
+      <c r="G113" s="14"/>
+      <c r="H113" s="15"/>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B114" s="14"/>
-      <c r="C114" s="15"/>
-      <c r="D114" s="15"/>
-      <c r="E114" s="15"/>
-      <c r="F114" s="15"/>
-      <c r="G114" s="15"/>
-      <c r="H114" s="16"/>
+      <c r="B114" s="13"/>
+      <c r="C114" s="14"/>
+      <c r="D114" s="14"/>
+      <c r="E114" s="14"/>
+      <c r="F114" s="14"/>
+      <c r="G114" s="14"/>
+      <c r="H114" s="15"/>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B115" s="14"/>
-      <c r="C115" s="15"/>
-      <c r="D115" s="15"/>
-      <c r="E115" s="15"/>
-      <c r="F115" s="15"/>
-      <c r="G115" s="15"/>
-      <c r="H115" s="16"/>
+      <c r="B115" s="13"/>
+      <c r="C115" s="14"/>
+      <c r="D115" s="14"/>
+      <c r="E115" s="14"/>
+      <c r="F115" s="14"/>
+      <c r="G115" s="14"/>
+      <c r="H115" s="15"/>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B116" s="17"/>
-      <c r="C116" s="18"/>
-      <c r="D116" s="18"/>
-      <c r="E116" s="18"/>
-      <c r="F116" s="18"/>
-      <c r="G116" s="18"/>
-      <c r="H116" s="19"/>
+      <c r="B116" s="16"/>
+      <c r="C116" s="17"/>
+      <c r="D116" s="17"/>
+      <c r="E116" s="17"/>
+      <c r="F116" s="17"/>
+      <c r="G116" s="17"/>
+      <c r="H116" s="18"/>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
@@ -1729,18 +1695,12 @@
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B121" s="4"/>
-      <c r="C121" s="20"/>
-      <c r="D121" s="20"/>
-      <c r="E121" s="20"/>
       <c r="F121" s="5"/>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B122" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C122" s="20"/>
-      <c r="D122" s="20"/>
-      <c r="E122" s="20"/>
       <c r="F122" s="5"/>
       <c r="G122" t="s">
         <v>22</v>
@@ -1753,34 +1713,22 @@
       <c r="B123" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C123" s="20"/>
-      <c r="D123" s="20"/>
-      <c r="E123" s="20"/>
       <c r="F123" s="5"/>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B124" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C124" s="20"/>
-      <c r="D124" s="20"/>
-      <c r="E124" s="20"/>
       <c r="F124" s="5"/>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B125" s="4"/>
-      <c r="C125" s="20"/>
-      <c r="D125" s="20"/>
-      <c r="E125" s="20"/>
       <c r="F125" s="5"/>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B126" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C126" s="20"/>
-      <c r="D126" s="20"/>
-      <c r="E126" s="20"/>
       <c r="F126" s="5"/>
       <c r="G126" t="s">
         <v>22</v>
@@ -1791,9 +1739,6 @@
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B127" s="4"/>
-      <c r="C127" s="20"/>
-      <c r="D127" s="20"/>
-      <c r="E127" s="20"/>
       <c r="F127" s="5"/>
       <c r="H127" t="s">
         <v>48</v>
@@ -1803,9 +1748,6 @@
       <c r="B128" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C128" s="20"/>
-      <c r="D128" s="20"/>
-      <c r="E128" s="20"/>
       <c r="F128" s="5"/>
       <c r="H128" t="s">
         <v>46</v>

</xml_diff>